<commit_message>
📚 Actualización de contenido académico - 2026-02-23 21:17
</commit_message>
<xml_diff>
--- a/03-week/01-session/Book1.xlsx
+++ b/03-week/01-session/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\Sena\ADSO-3239137\03-week\01-session\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88E7B102-8908-4957-B55F-FAC96B1008BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C0EF28-8851-4A94-8E6A-0E6A84AF9C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="7" xr2:uid="{3DCE18F1-D96C-414B-BE51-27DEC85764DC}"/>
   </bookViews>
@@ -27,6 +27,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escenario_1!$A$1:$I$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Escenario_2!$A$1:$I$116</definedName>
     <definedName name="data_aprendiz">Aprendiz!$A$2:$E$24</definedName>
+    <definedName name="data_ficha">Ficha_ADSO!$A$1:$C$10</definedName>
+    <definedName name="data_matricula_tema">matricula_tema!$A$6:$C$10</definedName>
+    <definedName name="list_matricula_tema">matricula_tema!$A$6:$A$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,8 +51,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="217">
   <si>
     <t>Código</t>
   </si>
@@ -731,7 +756,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -741,6 +766,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -782,7 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -794,6 +825,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6507,7 +6539,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="193" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6528,7 +6560,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>3239137</v>
+        <v>4324325</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -6552,7 +6584,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>3239137</v>
+        <v>4324325</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>31</v>
@@ -6576,7 +6608,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3239137</v>
+        <v>4324325</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>39</v>
@@ -6600,7 +6632,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>3239137</v>
+        <v>4324325</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>99</v>
@@ -6612,7 +6644,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>3239137</v>
+        <v>3221324</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>103</v>
@@ -6624,7 +6656,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>3239137</v>
+        <v>4324325</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>107</v>
@@ -6647,7 +6679,7 @@
   <dimension ref="A5:C10"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="256" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6701,7 +6733,7 @@
         <v>214</v>
       </c>
       <c r="B9" s="3">
-        <v>3239137</v>
+        <v>4324325</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -6725,30 +6757,177 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C213EDAD-6CA0-4065-AF28-DDEC1F9AEF80}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" zoomScale="228" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>216</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="str">
+        <f>CONCATENATE("Ficha: ",COUNTIF(data_ficha, C2))</f>
+        <v>Ficha: 5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="7">
+        <f>VLOOKUP(B2,data_matricula_tema,2,FALSE)</f>
+        <v>4324325</v>
+      </c>
+      <c r="D2" s="7" t="str" cm="1">
+        <f t="array" ref="D2:D6">_xlfn._xlws.FILTER(
+    INDEX(data_aprendiz,,2),
+    ISNUMBER(
+        MATCH(
+            INDEX(data_aprendiz,,1),
+            _xlfn._xlws.FILTER(Ficha_ADSO!B:B, Ficha_ADSO!A:A=C2),
+            0
+        )
+    )
+)</f>
+        <v>Luis Torres</v>
+      </c>
+      <c r="E2">
+        <f>VLOOKUP(B2,data_matricula_tema,2,FALSE)</f>
+        <v>4324325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="7">
+        <f>VLOOKUP(B3,data_matricula_tema,2,FALSE)</f>
+        <v>4324325</v>
+      </c>
+      <c r="D3" s="7" t="str">
+        <v>Carlos Peña</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="7">
+        <f>VLOOKUP(B4,data_matricula_tema,2,FALSE)</f>
+        <v>4324325</v>
+      </c>
+      <c r="D4" s="7" t="str">
+        <v>Juan Martínez</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" s="7">
+        <f>VLOOKUP(B5,data_matricula_tema,2,FALSE)</f>
+        <v>4324325</v>
+      </c>
+      <c r="D5" s="7" t="str">
+        <v>Isabella León</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="7">
+        <f>VLOOKUP(B6,data_matricula_tema,2,FALSE)</f>
+        <v>4324325</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <v>Mariana Beltrán Goméz</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7" t="e">
+        <f>VLOOKUP(B7,data_matricula_tema,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="e">
+        <f>VLOOKUP(B8,data_matricula_tema,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7" t="e">
+        <f>VLOOKUP(B9,data_matricula_tema,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="7" t="e">
+        <f>VLOOKUP(B10,data_matricula_tema,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{E5F4BF6B-3119-419B-B2CC-44C391C44D31}">
+      <formula1>list_matricula_tema</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>